<commit_message>
added only mutated xlsx
</commit_message>
<xml_diff>
--- a/result/interactions_download/Burkitt_lymphoma_precog.xlsx
+++ b/result/interactions_download/Burkitt_lymphoma_precog.xlsx
@@ -36,24 +36,24 @@
     <t xml:space="preserve">CHD4</t>
   </si>
   <si>
+    <t xml:space="preserve">ORF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBXW7</t>
+  </si>
+  <si>
     <t xml:space="preserve">NON_ORF</t>
   </si>
   <si>
-    <t xml:space="preserve">ECT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FBXW7</t>
-  </si>
-  <si>
     <t xml:space="preserve">KIF20A</t>
   </si>
   <si>
@@ -84,6 +84,9 @@
     <t xml:space="preserve">MTOR</t>
   </si>
   <si>
+    <t xml:space="preserve">BOTH</t>
+  </si>
+  <si>
     <t xml:space="preserve">MYO5A</t>
   </si>
   <si>
@@ -151,9 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">GLG1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOTH</t>
   </si>
   <si>
     <t xml:space="preserve">PPP1R9A</t>
@@ -1063,7 +1063,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" t="n">
         <v>-2.162</v>
@@ -1080,10 +1080,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
         <v>2.033</v>
@@ -1123,7 +1123,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
         <v>2.389</v>
@@ -1143,7 +1143,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
         <v>-2.758</v>
@@ -1183,7 +1183,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C10" t="n">
         <v>1.996</v>
@@ -1203,7 +1203,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C11" t="n">
         <v>-2.989</v>
@@ -1223,7 +1223,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C12" t="n">
         <v>-2.173</v>
@@ -1243,7 +1243,7 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C13" t="n">
         <v>2.028</v>
@@ -1283,7 +1283,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C15" t="n">
         <v>2.167</v>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C16" t="n">
         <v>-2.061</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -1340,10 +1340,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C18" t="n">
         <v>-3.031</v>
@@ -1360,10 +1360,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C19" t="n">
         <v>-2.196</v>
@@ -1380,10 +1380,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C20" t="n">
         <v>2.132</v>
@@ -1400,10 +1400,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C21" t="n">
         <v>2.398</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C22" t="n">
         <v>-3.348</v>
@@ -1440,10 +1440,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C23" t="n">
         <v>-3.255</v>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -1480,10 +1480,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C25" t="n">
         <v>2.123</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C26" t="n">
         <v>-2.387</v>
@@ -1520,10 +1520,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C27" t="n">
         <v>2.107</v>
@@ -1540,10 +1540,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C28" t="n">
         <v>-2.334</v>
@@ -1560,10 +1560,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C29" t="n">
         <v>-2.169</v>
@@ -1580,10 +1580,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C30" t="n">
         <v>2.127</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -1620,10 +1620,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C32" t="n">
         <v>-2.133</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
@@ -1720,10 +1720,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C37" t="n">
         <v>-2.582</v>
@@ -1740,10 +1740,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="C38" t="n">
         <v>2.066</v>
@@ -1783,7 +1783,7 @@
         <v>48</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C40" t="n">
         <v>-3.051</v>
@@ -1803,7 +1803,7 @@
         <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C41" t="n">
         <v>-1.97</v>
@@ -1823,7 +1823,7 @@
         <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C42" t="n">
         <v>2.612</v>
@@ -1843,7 +1843,7 @@
         <v>51</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C43" t="n">
         <v>-2.094</v>
@@ -1863,7 +1863,7 @@
         <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C44" t="n">
         <v>-2.184</v>
@@ -1903,7 +1903,7 @@
         <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C46" t="n">
         <v>2.337</v>
@@ -1923,7 +1923,7 @@
         <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C47" t="n">
         <v>-2.474</v>
@@ -1943,7 +1943,7 @@
         <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C48" t="n">
         <v>1.995</v>
@@ -1963,7 +1963,7 @@
         <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C49" t="n">
         <v>2.155</v>
@@ -2063,7 +2063,7 @@
         <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C54" t="n">
         <v>2.2</v>
@@ -2103,7 +2103,7 @@
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C56" t="n">
         <v>-3.075</v>
@@ -2143,7 +2143,7 @@
         <v>66</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C58" t="n">
         <v>-2.317</v>
@@ -2163,7 +2163,7 @@
         <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C59" t="n">
         <v>2.306</v>
@@ -2183,7 +2183,7 @@
         <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C60" t="n">
         <v>-2.08</v>
@@ -2263,7 +2263,7 @@
         <v>72</v>
       </c>
       <c r="B64" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C64" t="n">
         <v>2.019</v>
@@ -2283,7 +2283,7 @@
         <v>73</v>
       </c>
       <c r="B65" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C65" t="n">
         <v>-2.776</v>
@@ -2303,7 +2303,7 @@
         <v>74</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C66" t="n">
         <v>-2.209</v>
@@ -2463,7 +2463,7 @@
         <v>82</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C74" t="n">
         <v>1.991</v>
@@ -2523,7 +2523,7 @@
         <v>85</v>
       </c>
       <c r="B77" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C77" t="n">
         <v>2.076</v>
@@ -2543,7 +2543,7 @@
         <v>86</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C78" t="n">
         <v>2.063</v>
@@ -2563,7 +2563,7 @@
         <v>87</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C79" t="n">
         <v>2.088</v>
@@ -2663,7 +2663,7 @@
         <v>92</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C84" t="n">
         <v>2.231</v>
@@ -2743,7 +2743,7 @@
         <v>96</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C88" t="n">
         <v>2.541</v>
@@ -2763,7 +2763,7 @@
         <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C89" t="n">
         <v>-2.096</v>
@@ -2783,7 +2783,7 @@
         <v>98</v>
       </c>
       <c r="B90" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C90" t="n">
         <v>2.305</v>
@@ -2803,7 +2803,7 @@
         <v>99</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C91" t="n">
         <v>-1.97</v>
@@ -2823,7 +2823,7 @@
         <v>100</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C92" t="n">
         <v>2.162</v>
@@ -2843,7 +2843,7 @@
         <v>101</v>
       </c>
       <c r="B93" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C93" t="n">
         <v>-3.96</v>
@@ -3003,7 +3003,7 @@
         <v>109</v>
       </c>
       <c r="B101" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C101" t="n">
         <v>-2.328</v>
@@ -3023,7 +3023,7 @@
         <v>110</v>
       </c>
       <c r="B102" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C102" t="n">
         <v>-2.293</v>
@@ -3043,7 +3043,7 @@
         <v>111</v>
       </c>
       <c r="B103" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C103" t="n">
         <v>-2.039</v>
@@ -3103,7 +3103,7 @@
         <v>114</v>
       </c>
       <c r="B106" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C106" t="n">
         <v>2.213</v>
@@ -3143,7 +3143,7 @@
         <v>116</v>
       </c>
       <c r="B108" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C108" t="n">
         <v>2.818</v>
@@ -3183,7 +3183,7 @@
         <v>118</v>
       </c>
       <c r="B110" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C110" t="n">
         <v>-2.069</v>
@@ -3263,7 +3263,7 @@
         <v>122</v>
       </c>
       <c r="B114" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C114" t="n">
         <v>-2.239</v>
@@ -3303,7 +3303,7 @@
         <v>124</v>
       </c>
       <c r="B116" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C116" t="n">
         <v>-2.017</v>
@@ -3323,7 +3323,7 @@
         <v>125</v>
       </c>
       <c r="B117" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C117" t="n">
         <v>-2.194</v>
@@ -3343,7 +3343,7 @@
         <v>126</v>
       </c>
       <c r="B118" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C118" t="n">
         <v>2.377</v>
@@ -3443,7 +3443,7 @@
         <v>131</v>
       </c>
       <c r="B123" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C123" t="n">
         <v>2.392</v>
@@ -3463,7 +3463,7 @@
         <v>132</v>
       </c>
       <c r="B124" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C124" t="n">
         <v>-2.78</v>
@@ -3483,7 +3483,7 @@
         <v>133</v>
       </c>
       <c r="B125" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C125" t="n">
         <v>2.232</v>
@@ -3543,7 +3543,7 @@
         <v>136</v>
       </c>
       <c r="B128" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C128" t="n">
         <v>-2.094</v>
@@ -3603,7 +3603,7 @@
         <v>139</v>
       </c>
       <c r="B131" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C131" t="n">
         <v>2.743</v>
@@ -3683,7 +3683,7 @@
         <v>143</v>
       </c>
       <c r="B135" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C135" t="n">
         <v>2.112</v>
@@ -3703,7 +3703,7 @@
         <v>144</v>
       </c>
       <c r="B136" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C136" t="n">
         <v>-2.096</v>
@@ -3763,7 +3763,7 @@
         <v>147</v>
       </c>
       <c r="B139" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="C139" t="n">
         <v>2.157</v>
@@ -3783,7 +3783,7 @@
         <v>148</v>
       </c>
       <c r="B140" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C140" t="n">
         <v>-2.329</v>
@@ -3803,7 +3803,7 @@
         <v>149</v>
       </c>
       <c r="B141" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C141" t="n">
         <v>-1.96</v>
@@ -3923,7 +3923,7 @@
         <v>155</v>
       </c>
       <c r="B147" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C147" t="n">
         <v>-2.723</v>
@@ -3963,7 +3963,7 @@
         <v>157</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C149" t="n">
         <v>-2.642</v>
@@ -4003,7 +4003,7 @@
         <v>159</v>
       </c>
       <c r="B151" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C151" t="n">
         <v>2.513</v>
@@ -4043,7 +4043,7 @@
         <v>161</v>
       </c>
       <c r="B153" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C153" t="n">
         <v>-1.996</v>
@@ -4063,7 +4063,7 @@
         <v>162</v>
       </c>
       <c r="B154" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C154" t="n">
         <v>2.096</v>
@@ -4083,7 +4083,7 @@
         <v>163</v>
       </c>
       <c r="B155" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C155" t="n">
         <v>2.065</v>
@@ -4103,7 +4103,7 @@
         <v>164</v>
       </c>
       <c r="B156" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C156" t="n">
         <v>-2.025</v>
@@ -4123,7 +4123,7 @@
         <v>165</v>
       </c>
       <c r="B157" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C157" t="n">
         <v>-2.528</v>
@@ -4143,7 +4143,7 @@
         <v>166</v>
       </c>
       <c r="B158" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C158" t="n">
         <v>-1.983</v>
@@ -4183,7 +4183,7 @@
         <v>168</v>
       </c>
       <c r="B160" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C160" t="n">
         <v>2.287</v>
@@ -4203,7 +4203,7 @@
         <v>169</v>
       </c>
       <c r="B161" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C161" t="n">
         <v>-2.051</v>
@@ -4223,7 +4223,7 @@
         <v>170</v>
       </c>
       <c r="B162" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C162" t="n">
         <v>2.138</v>
@@ -4243,7 +4243,7 @@
         <v>171</v>
       </c>
       <c r="B163" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C163" t="n">
         <v>2.126</v>
@@ -4263,7 +4263,7 @@
         <v>172</v>
       </c>
       <c r="B164" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C164" t="n">
         <v>-1.976</v>
@@ -4283,7 +4283,7 @@
         <v>173</v>
       </c>
       <c r="B165" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C165" t="n">
         <v>2.351</v>
@@ -4303,7 +4303,7 @@
         <v>174</v>
       </c>
       <c r="B166" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C166" t="n">
         <v>2.064</v>
@@ -4323,7 +4323,7 @@
         <v>175</v>
       </c>
       <c r="B167" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C167" t="n">
         <v>2.294</v>
@@ -4343,7 +4343,7 @@
         <v>176</v>
       </c>
       <c r="B168" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C168" t="n">
         <v>2.097</v>
@@ -4363,7 +4363,7 @@
         <v>177</v>
       </c>
       <c r="B169" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C169" t="n">
         <v>2.064</v>
@@ -4403,7 +4403,7 @@
         <v>179</v>
       </c>
       <c r="B171" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C171" t="n">
         <v>-2.925</v>
@@ -4423,7 +4423,7 @@
         <v>180</v>
       </c>
       <c r="B172" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C172" t="n">
         <v>-2.218</v>
@@ -4443,7 +4443,7 @@
         <v>181</v>
       </c>
       <c r="B173" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C173" t="n">
         <v>2.478</v>
@@ -4463,7 +4463,7 @@
         <v>182</v>
       </c>
       <c r="B174" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C174" t="n">
         <v>2.023</v>
@@ -4483,7 +4483,7 @@
         <v>183</v>
       </c>
       <c r="B175" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C175" t="n">
         <v>-2.242</v>
@@ -4503,7 +4503,7 @@
         <v>184</v>
       </c>
       <c r="B176" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C176" t="n">
         <v>2.008</v>
@@ -4523,7 +4523,7 @@
         <v>185</v>
       </c>
       <c r="B177" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C177" t="n">
         <v>2.336</v>
@@ -4543,7 +4543,7 @@
         <v>186</v>
       </c>
       <c r="B178" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C178" t="n">
         <v>-4.454</v>
@@ -4563,7 +4563,7 @@
         <v>187</v>
       </c>
       <c r="B179" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C179" t="n">
         <v>-2.028</v>
@@ -4823,7 +4823,7 @@
         <v>200</v>
       </c>
       <c r="B192" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C192" t="n">
         <v>-3.017</v>
@@ -4963,7 +4963,7 @@
         <v>207</v>
       </c>
       <c r="B199" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C199" t="n">
         <v>-3.391</v>
@@ -5003,7 +5003,7 @@
         <v>209</v>
       </c>
       <c r="B201" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C201" t="n">
         <v>-2.655</v>
@@ -5165,7 +5165,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -5250,10 +5250,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19">
@@ -5261,12 +5261,12 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>213</v>
@@ -5274,7 +5274,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
         <v>214</v>
@@ -5365,7 +5365,7 @@
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33">
@@ -5397,7 +5397,7 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37">
@@ -5410,7 +5410,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B38" t="s">
         <v>16</v>
@@ -5466,7 +5466,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
         <v>17</v>
@@ -5514,7 +5514,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
@@ -5573,7 +5573,7 @@
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59">
@@ -5586,7 +5586,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B60" t="s">
         <v>22</v>
@@ -5605,15 +5605,15 @@
         <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64">
@@ -5621,15 +5621,15 @@
         <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66">
@@ -5637,12 +5637,12 @@
         <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B67" t="s">
         <v>213</v>
@@ -5650,7 +5650,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B68" t="s">
         <v>6</v>
@@ -5658,7 +5658,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -5666,7 +5666,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B70" t="s">
         <v>212</v>
@@ -5677,7 +5677,7 @@
         <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72">
@@ -5685,20 +5685,20 @@
         <v>6</v>
       </c>
       <c r="B72" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B74" t="s">
         <v>214</v>
@@ -5706,7 +5706,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B75" t="s">
         <v>214</v>
@@ -5714,7 +5714,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B76" t="s">
         <v>214</v>
@@ -5725,20 +5725,20 @@
         <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B79" t="s">
         <v>10</v>
@@ -5749,7 +5749,7 @@
         <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="81">
@@ -5757,7 +5757,7 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82">
@@ -5765,7 +5765,7 @@
         <v>6</v>
       </c>
       <c r="B82" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83">
@@ -5773,15 +5773,15 @@
         <v>15</v>
       </c>
       <c r="B83" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B84" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85">
@@ -5789,7 +5789,7 @@
         <v>15</v>
       </c>
       <c r="B85" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="86">
@@ -5797,7 +5797,7 @@
         <v>215</v>
       </c>
       <c r="B86" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87">
@@ -5805,12 +5805,12 @@
         <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B88" t="s">
         <v>14</v>
@@ -5818,10 +5818,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B89" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="90">
@@ -5829,7 +5829,7 @@
         <v>215</v>
       </c>
       <c r="B90" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="91">
@@ -5837,7 +5837,7 @@
         <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="92">
@@ -5845,7 +5845,7 @@
         <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="93">
@@ -5853,12 +5853,12 @@
         <v>214</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B94" t="s">
         <v>15</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B95" t="s">
         <v>8</v>
@@ -5874,7 +5874,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B96" t="s">
         <v>13</v>
@@ -5882,7 +5882,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B97" t="s">
         <v>215</v>
@@ -5890,7 +5890,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B98" t="s">
         <v>15</v>
@@ -5898,15 +5898,15 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B99" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B100" t="s">
         <v>8</v>
@@ -5914,7 +5914,7 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B101" t="s">
         <v>13</v>
@@ -6005,7 +6005,7 @@
         <v>54</v>
       </c>
       <c r="B112" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="113">
@@ -6013,7 +6013,7 @@
         <v>56</v>
       </c>
       <c r="B113" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="114">
@@ -6034,7 +6034,7 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B116" t="s">
         <v>60</v>
@@ -6050,7 +6050,7 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B118" t="s">
         <v>63</v>
@@ -6074,7 +6074,7 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B121" t="s">
         <v>68</v>
@@ -6106,7 +6106,7 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B125" t="s">
         <v>76</v>
@@ -6125,7 +6125,7 @@
         <v>82</v>
       </c>
       <c r="B127" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="128">
@@ -6197,7 +6197,7 @@
         <v>121</v>
       </c>
       <c r="B136" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137">
@@ -6218,7 +6218,7 @@
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B139" t="s">
         <v>141</v>
@@ -6237,7 +6237,7 @@
         <v>144</v>
       </c>
       <c r="B141" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142">

</xml_diff>